<commit_message>
added before hook in codecept, implemented xpath for demoqa.com
</commit_message>
<xml_diff>
--- a/xml-path/xml-prac.xlsx
+++ b/xml-path/xml-prac.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\xml-path\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\js-leetcode\xml-path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496EAA69-F41E-4F3A-8EB5-98838AF19B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16B199B-2575-443F-890B-E22ED06136C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4472C447-099B-4BE2-816E-2EABAC951C49}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4472C447-099B-4BE2-816E-2EABAC951C49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="164">
   <si>
     <t>Xpath Practice</t>
   </si>
@@ -692,13 +693,343 @@
   </si>
   <si>
     <t>//table/tbody/tr/td[text()='Alice']/following::tr/td[1]</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>practice.html</t>
+  </si>
+  <si>
+    <t>//label[@id='userName-label']//following::div[1]//input</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/text-box</t>
+  </si>
+  <si>
+    <t>Selecting input with label name</t>
+  </si>
+  <si>
+    <t>Selecting submit button</t>
+  </si>
+  <si>
+    <t>//button[@id='submit']</t>
+  </si>
+  <si>
+    <t>Selecting textarea using contains</t>
+  </si>
+  <si>
+    <t>//textarea[contains(@placeholder,'Current Address')]</t>
+  </si>
+  <si>
+    <t>Selecting textarea using label text and axes</t>
+  </si>
+  <si>
+    <t>//label[text()='Current Address']//parent::div//following-sibling::div//textarea</t>
+  </si>
+  <si>
+    <t>Selecting SVG element inside a div</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'header-right')]//*[local-name()='svg']</t>
+  </si>
+  <si>
+    <t>Selecting li which has a span with text 'Notes'</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Notes') and @class='rct-title']//ancestor::li[1]</t>
+  </si>
+  <si>
+    <t>Selecting radio input which is not disabled</t>
+  </si>
+  <si>
+    <t>//input[@type='radio' and not(@disabled)]</t>
+  </si>
+  <si>
+    <t>Selecting radio input which is disabled</t>
+  </si>
+  <si>
+    <t>//input[@type='radio' and @disabled]</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/radio-button</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/checkbox</t>
+  </si>
+  <si>
+    <t>Selecting the first div after a div containing text 'like the site'</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'like the site')]//following::div[1]</t>
+  </si>
+  <si>
+    <t>//label[text()='Yes']//preceding::input[1]</t>
+  </si>
+  <si>
+    <t>Selecting all column header</t>
+  </si>
+  <si>
+    <t>//div[@role='columnheader']</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/webtables</t>
+  </si>
+  <si>
+    <t>Selecting column header which has text 'Email'</t>
+  </si>
+  <si>
+    <t>Selecting a input which is preceding to label that has a text 'Yes'</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Email')]//parent::div[@role='columnheader']</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'rt-tbody')]//descendant::div[1]</t>
+  </si>
+  <si>
+    <t>Selecting the first row in the table body</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'rt-tbody')]//div[text()='Alden']//parent::div//div[4]</t>
+  </si>
+  <si>
+    <t>Selecting email of the person with name 'Alden'</t>
+  </si>
+  <si>
+    <t>Selecting the edit button of the row which has first name 'Kierra'</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'rt-tbody')]//div[text()='Kierra']//following-sibling::div//div[@class='action-buttons']/span[contains(@title,'Edit')]</t>
+  </si>
+  <si>
+    <t>Select the salary of th 3rd row</t>
+  </si>
+  <si>
+    <t>(//div[contains(@class,'rt-tbody')]//div[@role='row'])[3]//div[5]</t>
+  </si>
+  <si>
+    <t>Selecting non empty rows in the table body</t>
+  </si>
+  <si>
+    <t>//span[string-length(text())=0]//ancestor::div[@role='row']</t>
+  </si>
+  <si>
+    <t>(//span[string-length(text())=0]//ancestor::div[@role='row'])[last()]//div[4]</t>
+  </si>
+  <si>
+    <t>Selecting email of the row before first empty row</t>
+  </si>
+  <si>
+    <t>Selecting rows which has salary &gt; 5000</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'rt-tr') and @role='row']//following::div[number(text())&gt;5000 and position()=4]</t>
+  </si>
+  <si>
+    <t>Selecting all div that starts with class col-md-3</t>
+  </si>
+  <si>
+    <t>//div[starts-with(@class,'col-md-3')]</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/automation-practice-form</t>
+  </si>
+  <si>
+    <t>Selecting second radio button in gender section</t>
+  </si>
+  <si>
+    <t>//div[@id='genterWrapper']//div[text()='Gender']//following-sibling::div/div[position()=2]//input</t>
+  </si>
+  <si>
+    <t>//input[@id='firstName']//preceding::label</t>
+  </si>
+  <si>
+    <t>Selecting label of the input firstName</t>
+  </si>
+  <si>
+    <t>//input[@minlength and @maxlength]</t>
+  </si>
+  <si>
+    <t>Selecting input which has both minlength and maxlength attribute</t>
+  </si>
+  <si>
+    <t>Selecting input with type file inside user form</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[@type = 'file' and @id='uploadPicture']</t>
+  </si>
+  <si>
+    <t>//img[not(@alt)]//preceding::p[contains(text(),'Valid image')]</t>
+  </si>
+  <si>
+    <t>Selecting image that has not alt and is after a p with text 'Valid image'</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/broken</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[@id='userEmail']//parent::div</t>
+  </si>
+  <si>
+    <t>Selecting parent div of the email input</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//label[text()='Reading']//preceding-sibling::input[@type='checkbox']</t>
+  </si>
+  <si>
+    <t>Selecting checbox of label 'Reading'</t>
+  </si>
+  <si>
+    <t>Selecting textarea with placeholder 'Current Address'</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//textarea[@placeholder='Current Address']</t>
+  </si>
+  <si>
+    <t>Selecting button using aria-label</t>
+  </si>
+  <si>
+    <t>//button[@aria-label='Toggle']</t>
+  </si>
+  <si>
+    <t>Selecting button using lower case attriubutes</t>
+  </si>
+  <si>
+    <t>//button[translate(@title,'T','t')='toggle']</t>
+  </si>
+  <si>
+    <t>Selecting all input with autocomplete off</t>
+  </si>
+  <si>
+    <t>Selecting div with inline style</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//div[@style]</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[@autocomplete='off']</t>
+  </si>
+  <si>
+    <t>Selecting input which is disabled</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[@disabled]</t>
+  </si>
+  <si>
+    <t>Selecting input of type checkbox and value less than 3</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[@type='checkbox' and @value&lt;3]</t>
+  </si>
+  <si>
+    <t>Selecting label with attribute for that starts with 'hobbies'</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//label[starts-with(@for,'hobbies')]</t>
+  </si>
+  <si>
+    <t>Selecting inputs which has id of length&gt;10</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[string-length(@id)&gt;10]</t>
+  </si>
+  <si>
+    <t>//div[@id='stateCity-wrapper']/preceding-sibling::div[1]</t>
+  </si>
+  <si>
+    <t>Selects the previous div of the div with id stateCity-wrapper</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'wrapper') and not(contains(@class,'form-wrapper'))]</t>
+  </si>
+  <si>
+    <t>Selecting all divs that contains wrapper in class but not form-wrapper</t>
+  </si>
+  <si>
+    <t>Selecting input with both required and pattern attribute</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//input[@required and @pattern]</t>
+  </si>
+  <si>
+    <t>Selecting last checkbox in hobbies column</t>
+  </si>
+  <si>
+    <t>//form[@id='userForm']//div[@id='hobbiesWrapper']//div[last()]/input[@type='checkbox']</t>
+  </si>
+  <si>
+    <t>Selecting second div that contains class col-md-9</t>
+  </si>
+  <si>
+    <t>(//div[contains(@class,'col-md-9')])[2]</t>
+  </si>
+  <si>
+    <t>Selecting button with text Previous and is disabled</t>
+  </si>
+  <si>
+    <t>//div[@class='pagination-bottom']//button[text()='Previous' and @disabled]</t>
+  </si>
+  <si>
+    <t>https://demoqa/webtables</t>
+  </si>
+  <si>
+    <t>//div[text()='Cierra']/following-sibling::div[1]</t>
+  </si>
+  <si>
+    <t>htttps://demoqa/webtables</t>
+  </si>
+  <si>
+    <t>Selecting the first sibling div of a div with text Cierra</t>
+  </si>
+  <si>
+    <t>Selecting the department where salary &gt;=10k</t>
+  </si>
+  <si>
+    <t>//div[@role='rowgroup']//div[@role='row']/div[number(text())&gt;=10000]//following-sibling::div[1]</t>
+  </si>
+  <si>
+    <t>Selecting input with placeholder 'Type to search'</t>
+  </si>
+  <si>
+    <t>//input[contains(@placeholder,'Type to search')]</t>
+  </si>
+  <si>
+    <t>//span[text()='Notes']/ancestor::li[1]/following-sibling::li//span[text()='Commands']</t>
+  </si>
+  <si>
+    <t>Selecting the sibling checkbox of checkbox with text Notes</t>
+  </si>
+  <si>
+    <t>https://demoqa/checkbox</t>
+  </si>
+  <si>
+    <t>//div[@id='tree-node']//ol//child::li[contains(@class,'rct-node-parent') and not(contains(@class,'rct-node-expanded'))]</t>
+  </si>
+  <si>
+    <t>Selecting all collapsed nodes</t>
+  </si>
+  <si>
+    <t>Selecting Angular node from React Node</t>
+  </si>
+  <si>
+    <t>//div[@id='tree-node']//li[.//span[text()='React']]/following-sibling::li[1]//span[text()='Angular']</t>
+  </si>
+  <si>
+    <t>//label//following-sibling::input[@lang='en']</t>
+  </si>
+  <si>
+    <t>Selecting input with lang attribute en and that is a sibling of a label</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/upload-download</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +1058,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -745,23 +1092,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1094,45 +1450,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E72B32-B2C1-4FA7-BC72-F187CB33496E}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="56.44140625" customWidth="1"/>
-    <col min="3" max="3" width="65.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="60.08984375" customWidth="1"/>
+    <col min="3" max="3" width="108.26953125" customWidth="1"/>
+    <col min="4" max="4" width="39.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6">
+    <row r="1" spans="1:13" ht="16">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1145,6 +1505,9 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
@@ -1156,6 +1519,9 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
@@ -1167,6 +1533,9 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6">
@@ -1178,6 +1547,9 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7">
@@ -1189,6 +1561,9 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8">
@@ -1200,6 +1575,9 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9">
@@ -1211,16 +1589,22 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1233,16 +1617,22 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1255,6 +1645,9 @@
       <c r="C13" t="s">
         <v>25</v>
       </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
@@ -1266,16 +1659,22 @@
       <c r="C14" t="s">
         <v>27</v>
       </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1288,8 +1687,11 @@
       <c r="C16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1299,8 +1701,11 @@
       <c r="C17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1310,8 +1715,11 @@
       <c r="C18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1321,8 +1729,11 @@
       <c r="C19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1332,8 +1743,11 @@
       <c r="C20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1343,8 +1757,11 @@
       <c r="C21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1354,8 +1771,11 @@
       <c r="C22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1365,19 +1785,25 @@
       <c r="C23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1387,8 +1813,11 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1398,8 +1827,11 @@
       <c r="C26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1409,12 +1841,763 @@
       <c r="C27" t="s">
         <v>53</v>
       </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16">
+      <c r="B28" s="6">
+        <v>45936</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>141</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>143</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" t="s">
+        <v>151</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" t="s">
+        <v>154</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" t="s">
+        <v>160</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" t="s">
+        <v>161</v>
+      </c>
+      <c r="D77" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D30" r:id="rId1" xr:uid="{F2219569-A45E-40B8-8695-E79665FE28C1}"/>
+    <hyperlink ref="D31" r:id="rId2" xr:uid="{A0502E3E-A03B-4906-A044-0F317C872441}"/>
+    <hyperlink ref="D32" r:id="rId3" xr:uid="{6F2EC370-B13D-4F95-8F97-0DED2ECFE415}"/>
+    <hyperlink ref="D33" r:id="rId4" xr:uid="{073BF9CD-C5E7-4E0B-9217-4288C94F0994}"/>
+    <hyperlink ref="D34" r:id="rId5" xr:uid="{EBF1697B-0428-420F-9D83-0264C6681292}"/>
+    <hyperlink ref="D35" r:id="rId6" xr:uid="{1B191DC0-2415-48C7-878A-90763FD22A11}"/>
+    <hyperlink ref="D36" r:id="rId7" xr:uid="{B2EECDCE-C41A-40BB-BAE3-32F1FBF88375}"/>
+    <hyperlink ref="D37" r:id="rId8" xr:uid="{E527113D-0466-4A6D-ADD7-5DE885F8CF49}"/>
+    <hyperlink ref="D38" r:id="rId9" xr:uid="{7DC45F3D-ED65-49E9-937D-77BC6321676D}"/>
+    <hyperlink ref="D40" r:id="rId10" xr:uid="{FED5275D-D77A-428A-9F52-E674F97B3BF1}"/>
+    <hyperlink ref="D41" r:id="rId11" xr:uid="{34DA804F-D72D-4E28-B9E5-5A7D551ED343}"/>
+    <hyperlink ref="D42" r:id="rId12" xr:uid="{C5B71E04-FF21-45C8-A703-BE00442EAE24}"/>
+    <hyperlink ref="D43" r:id="rId13" xr:uid="{9F9C6047-8048-45B8-B7F4-DCA98F07994B}"/>
+    <hyperlink ref="D44" r:id="rId14" xr:uid="{0AC72807-94E7-47BC-9FC4-6975F3831389}"/>
+    <hyperlink ref="D45" r:id="rId15" xr:uid="{58C58307-17E9-45FD-82E4-2CC4FA71F1AF}"/>
+    <hyperlink ref="D46" r:id="rId16" xr:uid="{3C334844-1606-4AE2-96CF-93413B363377}"/>
+    <hyperlink ref="D47" r:id="rId17" xr:uid="{B97168DA-7D5A-42AC-9B9C-14AF997FAEF0}"/>
+    <hyperlink ref="D48" r:id="rId18" xr:uid="{F4ACC2A7-6C37-4722-86F4-F7B01FEF7DC6}"/>
+    <hyperlink ref="D49" r:id="rId19" xr:uid="{0002D2D4-938E-48E2-9267-8691A94F7F46}"/>
+    <hyperlink ref="D50" r:id="rId20" xr:uid="{FAB80745-9FAF-4E96-9AA9-4C10631D96FF}"/>
+    <hyperlink ref="D52" r:id="rId21" xr:uid="{663BC736-AB69-45D2-9CCC-C9A0CC3D2ACF}"/>
+    <hyperlink ref="D53" r:id="rId22" xr:uid="{B2826C94-6E1C-4124-819E-20AFB0D0BB5D}"/>
+    <hyperlink ref="D54" r:id="rId23" xr:uid="{F45160B0-11E5-469E-A7C8-9C3DD75A1E03}"/>
+    <hyperlink ref="D56" r:id="rId24" xr:uid="{032BD7A2-F7AE-44D3-B4AD-4AC2CF5BB9B5}"/>
+    <hyperlink ref="D58" r:id="rId25" xr:uid="{EE11C1A0-72E5-48AA-8459-5541DF27B8AB}"/>
+    <hyperlink ref="D59" r:id="rId26" xr:uid="{DF60BB7F-86E0-4A92-8159-C263A8CE29A7}"/>
+    <hyperlink ref="D60" r:id="rId27" xr:uid="{6D489124-14AA-405F-8976-D5D027D317D0}"/>
+    <hyperlink ref="D61" r:id="rId28" xr:uid="{BAF84ED9-F6C1-4703-82C4-9FAC65C383CA}"/>
+    <hyperlink ref="D62" r:id="rId29" xr:uid="{F7E8F406-685D-4CC9-A2C7-6984362B0C10}"/>
+    <hyperlink ref="D63" r:id="rId30" xr:uid="{CEFA83E2-EC57-4BFC-BD4B-2DBD58AF6DE2}"/>
+    <hyperlink ref="D64" r:id="rId31" xr:uid="{5BABC7F6-03C7-40E0-8C9E-422E155E6361}"/>
+    <hyperlink ref="D65" r:id="rId32" xr:uid="{9675437C-EAD4-445D-B9AB-7866E6665061}"/>
+    <hyperlink ref="D66" r:id="rId33" xr:uid="{949E0440-7701-46F0-8A96-65B9EF1694C8}"/>
+    <hyperlink ref="D67" r:id="rId34" xr:uid="{B69B0B87-8F6F-44B9-BD05-51502EFB08EE}"/>
+    <hyperlink ref="D68" r:id="rId35" xr:uid="{32E67A55-A2DB-4508-AB98-64BBCA1658FA}"/>
+    <hyperlink ref="D69" r:id="rId36" xr:uid="{664004CC-4CA0-4268-85D9-88717F844777}"/>
+    <hyperlink ref="D70" r:id="rId37" xr:uid="{AA5A0A6B-6CE4-41CB-9768-DF4503304BBD}"/>
+    <hyperlink ref="D73" r:id="rId38" xr:uid="{B24B1009-13FD-4C00-BC42-060C5F3371FC}"/>
+    <hyperlink ref="D72" r:id="rId39" xr:uid="{71A25569-21F4-4616-B82F-7D429A6BE673}"/>
+    <hyperlink ref="D74" r:id="rId40" xr:uid="{289E0F5C-CDC2-4BCC-BDF4-276E2F1F1BE5}"/>
+    <hyperlink ref="D75" r:id="rId41" xr:uid="{A8E06575-8799-4B27-A82C-508CF143608D}"/>
+    <hyperlink ref="D76" r:id="rId42" xr:uid="{0A1620F5-6F0A-4BC4-A634-24F292311A3A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>